<commit_message>
Updated report and reported results
</commit_message>
<xml_diff>
--- a/paper/risultati/risultati.xlsx
+++ b/paper/risultati/risultati.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Francesco\Documents\GitHub\mldl\paper\risultati\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{618894C2-93EA-4FC1-8FD7-0FD2D1A2644D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C85A229C-18D1-4450-A80E-2DFC63D599C4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>RGB Stage1 NOCAM @ 7</t>
   </si>
@@ -61,6 +61,12 @@
   </si>
   <si>
     <t>Warp Flow @ 5 5 tests</t>
+  </si>
+  <si>
+    <t>Two stream @ 16</t>
+  </si>
+  <si>
+    <t>Two stream @ 7</t>
   </si>
 </sst>
 </file>
@@ -104,9 +110,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -387,10 +394,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:F15"/>
+  <dimension ref="A2:F19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -448,7 +455,7 @@
         <v>44.83</v>
       </c>
       <c r="F5">
-        <f t="shared" ref="F4:F6" si="0">AVERAGE(B5:D5)</f>
+        <f t="shared" ref="F4:F18" si="0">AVERAGE(B5:D5)</f>
         <v>45.976666666666667</v>
       </c>
     </row>
@@ -483,6 +490,10 @@
       <c r="D8">
         <v>37.07</v>
       </c>
+      <c r="F8">
+        <f t="shared" si="0"/>
+        <v>38.79666666666666</v>
+      </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
@@ -497,6 +508,10 @@
       <c r="D9">
         <v>56.9</v>
       </c>
+      <c r="F9">
+        <f t="shared" si="0"/>
+        <v>56.32</v>
+      </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
@@ -511,6 +526,10 @@
       <c r="D11">
         <v>49.14</v>
       </c>
+      <c r="F11">
+        <f t="shared" si="0"/>
+        <v>51.723333333333336</v>
+      </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
@@ -525,6 +544,10 @@
       <c r="D12">
         <v>65.52</v>
       </c>
+      <c r="F12">
+        <f t="shared" si="0"/>
+        <v>66.666666666666671</v>
+      </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
@@ -539,12 +562,68 @@
       <c r="D14">
         <v>39.659999999999997</v>
       </c>
+      <c r="F14">
+        <f t="shared" si="0"/>
+        <v>40.520000000000003</v>
+      </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>9</v>
       </c>
-      <c r="B15" s="1"/>
+      <c r="B15" s="2">
+        <v>50.86</v>
+      </c>
+      <c r="C15">
+        <v>48.28</v>
+      </c>
+      <c r="D15">
+        <v>47.41</v>
+      </c>
+      <c r="F15">
+        <f t="shared" si="0"/>
+        <v>48.85</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>11</v>
+      </c>
+      <c r="B17">
+        <v>66.38</v>
+      </c>
+      <c r="C17">
+        <v>69.83</v>
+      </c>
+      <c r="D17">
+        <v>67.239999999999995</v>
+      </c>
+      <c r="E17" s="1"/>
+      <c r="F17">
+        <f t="shared" si="0"/>
+        <v>67.816666666666663</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>10</v>
+      </c>
+      <c r="B18">
+        <v>75</v>
+      </c>
+      <c r="C18">
+        <v>75</v>
+      </c>
+      <c r="D18">
+        <v>75</v>
+      </c>
+      <c r="F18">
+        <f t="shared" si="0"/>
+        <v>75</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F19" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>